<commit_message>
Add: add correct delta of expenses compared to previous 30 days
</commit_message>
<xml_diff>
--- a/data/data_example.xlsx
+++ b/data/data_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\solutions\learning_python\expense_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671C375D-D247-4CEB-81D4-EBBC8674C876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226DF38E-8EA4-4D57-B08D-7A04E0EDD316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" xr2:uid="{7A62D1F9-0105-4F41-8BB8-21CA3D721AF6}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="total" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">total!$A$1:$J$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">total!$A$1:$K$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>expense_type</t>
   </si>
@@ -71,9 +71,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>weekday</t>
-  </si>
-  <si>
     <t>english_translation</t>
   </si>
   <si>
@@ -93,6 +90,12 @@
   </si>
   <si>
     <t>rome</t>
+  </si>
+  <si>
+    <t>weekday_number</t>
+  </si>
+  <si>
+    <t>weekday_text</t>
   </si>
 </sst>
 </file>
@@ -445,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397426C9-9494-4E73-BF9B-2DE40DB1433B}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,10 +460,10 @@
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -480,19 +483,22 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>36526</v>
       </c>
@@ -500,7 +506,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -517,14 +523,18 @@
         <f t="shared" ref="G2:G6" si="2">WEEKDAY(A2, 2)</f>
         <v>6</v>
       </c>
-      <c r="H2" t="s">
-        <v>6</v>
+      <c r="H2" t="str">
+        <f>CHOOSE(WEEKDAY(A2, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>36526</v>
       </c>
@@ -532,7 +542,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>2.99</v>
@@ -549,14 +559,18 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H3" t="s">
-        <v>6</v>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H6" si="3">CHOOSE(WEEKDAY(A3, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Saturday</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>36526</v>
       </c>
@@ -564,7 +578,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>1.59</v>
@@ -581,14 +595,18 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H4" t="s">
-        <v>6</v>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>36526</v>
       </c>
@@ -596,7 +614,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>2.39</v>
@@ -613,14 +631,18 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H5" t="s">
-        <v>6</v>
+      <c r="H5" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>36526</v>
       </c>
@@ -628,7 +650,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <f>4.35/2</f>
@@ -646,11 +668,15 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H6" t="s">
-        <v>6</v>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>Saturday</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: add new data_example.xlsx file
</commit_message>
<xml_diff>
--- a/data/data_example.xlsx
+++ b/data/data_example.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\solutions\learning_python\expense_tracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226DF38E-8EA4-4D57-B08D-7A04E0EDD316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D030250C-76EF-4BD9-83A1-1A470AFE3EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="859" xr2:uid="{7A62D1F9-0105-4F41-8BB8-21CA3D721AF6}"/>
   </bookViews>
   <sheets>
-    <sheet name="total" sheetId="8" r:id="rId1"/>
+    <sheet name="total" sheetId="9" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">total!$A$1:$K$6</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>expense_type</t>
   </si>
@@ -56,46 +53,55 @@
     <t>expense_category</t>
   </si>
   <si>
+    <t>transportation</t>
+  </si>
+  <si>
     <t>store</t>
   </si>
   <si>
-    <t>lidl</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
+    <t>cleaning products</t>
+  </si>
+  <si>
     <t>month</t>
   </si>
   <si>
     <t>year</t>
   </si>
   <si>
-    <t>english_translation</t>
+    <t>weekday_number</t>
+  </si>
+  <si>
+    <t>weekday_text</t>
+  </si>
+  <si>
+    <t>months_text</t>
   </si>
   <si>
     <t>zucchini</t>
   </si>
   <si>
-    <t>muesly</t>
-  </si>
-  <si>
-    <t>cracker</t>
-  </si>
-  <si>
-    <t>orange juice</t>
-  </si>
-  <si>
-    <t>salami</t>
-  </si>
-  <si>
-    <t>rome</t>
-  </si>
-  <si>
-    <t>weekday_number</t>
-  </si>
-  <si>
-    <t>weekday_text</t>
+    <t>watermelon</t>
+  </si>
+  <si>
+    <t>window cleaner</t>
+  </si>
+  <si>
+    <t>detergent</t>
+  </si>
+  <si>
+    <t>butter</t>
+  </si>
+  <si>
+    <t>cocoa</t>
+  </si>
+  <si>
+    <t>train ticket</t>
+  </si>
+  <si>
+    <t>bus ticket</t>
   </si>
 </sst>
 </file>
@@ -447,20 +453,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397426C9-9494-4E73-BF9B-2DE40DB1433B}">
-  <dimension ref="A1:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB97080-BCC1-46F5-9840-552CC3734D33}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -477,206 +489,298 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>36526</v>
+        <v>43831</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>5.3</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E6" si="0">MONTH(A2)</f>
+        <f>MONTH(A2)</f>
         <v>1</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F6" si="1">YEAR(A2)</f>
-        <v>2000</v>
+        <f>YEAR(A2)</f>
+        <v>2020</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G6" si="2">WEEKDAY(A2, 2)</f>
-        <v>6</v>
+        <f>WEEKDAY(A2, 2)</f>
+        <v>3</v>
       </c>
       <c r="H2" t="str">
         <f>CHOOSE(WEEKDAY(A2, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
-        <v>Saturday</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
+        <v>Wednesday</v>
+      </c>
+      <c r="I2" t="str">
+        <f>TEXT(A2, "MMM")</f>
+        <v>Jan</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>36526</v>
+        <v>43831</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>2.99</v>
+        <v>0.79</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>MONTH(A3)</f>
         <v>1</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
-        <v>2000</v>
+        <f>YEAR(A3)</f>
+        <v>2020</v>
       </c>
       <c r="G3">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>WEEKDAY(A3, 2)</f>
+        <v>3</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H6" si="3">CHOOSE(WEEKDAY(A3, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
-        <v>Saturday</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
+        <f>CHOOSE(WEEKDAY(A3, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I3" t="str">
+        <f>TEXT(A3, "MMM")</f>
+        <v>Jan</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>36526</v>
+        <v>43831</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D4">
-        <v>1.59</v>
+        <v>0.95</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>MONTH(A4)</f>
         <v>1</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>2000</v>
+        <f>YEAR(A4)</f>
+        <v>2020</v>
       </c>
       <c r="G4">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>WEEKDAY(A4, 2)</f>
+        <v>3</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="3"/>
-        <v>Saturday</v>
-      </c>
-      <c r="I4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
+        <f>CHOOSE(WEEKDAY(A4, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I4" t="str">
+        <f>TEXT(A4, "MMM")</f>
+        <v>Jan</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>36526</v>
+        <v>43831</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D5">
-        <v>2.39</v>
+        <f>1.19/2</f>
+        <v>0.59499999999999997</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>MONTH(A5)</f>
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>2000</v>
+        <f>YEAR(A5)</f>
+        <v>2020</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>WEEKDAY(A5, 2)</f>
+        <v>3</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="3"/>
-        <v>Saturday</v>
-      </c>
-      <c r="I5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
+        <f>CHOOSE(WEEKDAY(A5, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I5" t="str">
+        <f>TEXT(A5, "MMM")</f>
+        <v>Jan</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>36526</v>
+        <v>43831</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <f>4.35/2</f>
-        <v>2.1749999999999998</v>
+        <v>0.99</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>MONTH(A6)</f>
         <v>1</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
-        <v>2000</v>
+        <f>YEAR(A6)</f>
+        <v>2020</v>
       </c>
       <c r="G6">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>WEEKDAY(A6, 2)</f>
+        <v>3</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="3"/>
-        <v>Saturday</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
+        <f>CHOOSE(WEEKDAY(A6, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I6" t="str">
+        <f>TEXT(A6, "MMM")</f>
+        <v>Jan</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>1.05</v>
+      </c>
+      <c r="E7">
+        <f>MONTH(A7)</f>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f>YEAR(A7)</f>
+        <v>2020</v>
+      </c>
+      <c r="G7">
+        <f>WEEKDAY(A7, 2)</f>
+        <v>3</v>
+      </c>
+      <c r="H7" t="str">
+        <f>CHOOSE(WEEKDAY(A7, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I7" t="str">
+        <f>TEXT(A7, "MMM")</f>
+        <v>Jan</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <f>MONTH(A8)</f>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f>YEAR(A8)</f>
+        <v>2020</v>
+      </c>
+      <c r="G8">
+        <f>WEEKDAY(A8, 2)</f>
+        <v>3</v>
+      </c>
+      <c r="H8" t="str">
+        <f>CHOOSE(WEEKDAY(A8, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I8" t="str">
+        <f>TEXT(A8, "MMM")</f>
+        <v>Jan</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <f>MONTH(A9)</f>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f>YEAR(A9)</f>
+        <v>2020</v>
+      </c>
+      <c r="G9">
+        <f>WEEKDAY(A9, 2)</f>
+        <v>3</v>
+      </c>
+      <c r="H9" t="str">
+        <f>CHOOSE(WEEKDAY(A9, 2), "Monday", "Tuesday","Wednesday", "Thursday", "Friday", "Saturday","Sunday")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="I9" t="str">
+        <f>TEXT(A9, "MMM")</f>
+        <v>Jan</v>
       </c>
     </row>
   </sheetData>

</xml_diff>